<commit_message>
task-4 + added react interface
</commit_message>
<xml_diff>
--- a/covid_19_data.xlsx
+++ b/covid_19_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>nome</t>
   </si>
@@ -22,6 +22,9 @@
     <t>totale</t>
   </si>
   <si>
+    <t>data</t>
+  </si>
+  <si>
     <t>Lombardia</t>
   </si>
   <si>
@@ -49,12 +52,12 @@
     <t>Friuli Venezia Giulia</t>
   </si>
   <si>
+    <t>Marche</t>
+  </si>
+  <si>
     <t>Liguria</t>
   </si>
   <si>
-    <t>Marche</t>
-  </si>
-  <si>
     <t>Abruzzo</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
   </si>
   <si>
     <t>Valle d'Aosta</t>
+  </si>
+  <si>
+    <t>2021-06-10T17:00:00</t>
   </si>
 </sst>
 </file>
@@ -437,238 +443,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>808683</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>838693</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>396053</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>422006</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>371776</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>385321</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>347320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>361871</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>326470</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>343947</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>237116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>251880</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>229037</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>242960</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>210993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>228621</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>105454</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>107299</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>99972</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>103301</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>98155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>103010</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>71640</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>74399</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>71354</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>73141</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>60925</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>67950</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>54876</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>56956</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>54638</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>56619</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>44132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>45640</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19">
-        <v>24258</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>26596</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20">
-        <v>13309</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>13625</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21">
-        <v>11041</v>
+        <v>11649</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>